<commit_message>
- Added function getWisdom to return a quote based upon inputs feeling & contect - Modified xls so that javascript is generated in the excel file
</commit_message>
<xml_diff>
--- a/Wisdom database.xlsx
+++ b/Wisdom database.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55bed276fccc9b95/Documents/2. Hanne/02. coding/ITCareerSwitch/Projects/Wisdom Supplies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\MijnRepository\WisdomSupplies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{959D2F38-543A-42FA-A2DB-5A2B787244C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BD540755-A69D-4A3D-B716-F86C3B78FFB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBACA2A2-456C-4260-95B3-1518FF77CCF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{859021F3-435E-49E2-A654-94E8C4143270}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{859021F3-435E-49E2-A654-94E8C4143270}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,24 +30,6 @@
     <t>anger</t>
   </si>
   <si>
-    <t>"Anger resolves nothing it only puts up your blood pressure."</t>
-  </si>
-  <si>
-    <t>"To be angry is to let others' mistakes punish yourself."</t>
-  </si>
-  <si>
-    <t>"I was angered, for I had no shoes. Then I met a man who had no feet."</t>
-  </si>
-  <si>
-    <t>"If you are patient in one moment of anger, you will escape a hundred days of sorrow."</t>
-  </si>
-  <si>
-    <t>"Anger and jealousy can no more bear to lose sight of their objects than love." </t>
-  </si>
-  <si>
-    <t>"Anger blows out the lamp of the mind."</t>
-  </si>
-  <si>
     <t>sad</t>
   </si>
   <si>
@@ -133,6 +115,24 @@
   </si>
   <si>
     <t>love</t>
+  </si>
+  <si>
+    <t>Anger blows out the lamp of the mind.</t>
+  </si>
+  <si>
+    <t>Anger resolves nothing it only puts up your blood pressure.</t>
+  </si>
+  <si>
+    <t>To be angry is to let others' mistakes punish yourself.</t>
+  </si>
+  <si>
+    <t>I was angered, for I had no shoes. Then I met a man who had no feet.</t>
+  </si>
+  <si>
+    <t>If you are patient in one moment of anger, you will escape a hundred days of sorrow.</t>
+  </si>
+  <si>
+    <t>Anger and jealousy can no more bear to lose sight of their objects than love.</t>
   </si>
 </sst>
 </file>
@@ -182,7 +182,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -198,7 +198,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -494,380 +494,480 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EBE504-7469-4B1A-8285-7C942805D0DE}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="149.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="89.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"if(feeling =='" &amp;A2 &amp;"' &amp;&amp; context == '"&amp;B2 &amp;"') {return '" &amp; D2 &amp; "';}"</f>
+        <v>if(feeling =='anger' &amp;&amp; context == 'work') {return 'Anger resolves nothing it only puts up your blood pressure.';}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="E3" t="str">
+        <f>"else if(feeling =='" &amp;A3 &amp;"' &amp;&amp; context == '"&amp;B3 &amp;"') {return '" &amp; D3 &amp; "';}"</f>
+        <v>else if(feeling =='anger' &amp;&amp; context == 'work') {return 'To be angry is to let others' mistakes punish yourself.';}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="str">
+        <f t="shared" ref="E4:E26" si="0">"else if(feeling =='" &amp;A4 &amp;"' &amp;&amp; context == '"&amp;B4 &amp;"') {return '" &amp; D4 &amp; "';}"</f>
+        <v>else if(feeling =='anger' &amp;&amp; context == 'family and friends') {return 'I was angered, for I had no shoes. Then I met a man who had no feet.';}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='anger' &amp;&amp; context == 'love') {return 'If you are patient in one moment of anger, you will escape a hundred days of sorrow.';}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='anger' &amp;&amp; context == 'love') {return 'Anger and jealousy can no more bear to lose sight of their objects than love.';}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='anger' &amp;&amp; context == 'love') {return 'Anger blows out the lamp of the mind.';}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='sad' &amp;&amp; context == 'love') {return 'Trying to avoid sadness is trying to avoid life.';}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='sad' &amp;&amp; context == 'love') {return 'What brings us to tears, will lead us to grace. Our pain is never wasted.';}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='sad' &amp;&amp; context == 'love') {return 'There are two medicines for all ills: time and silence.';}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='sad' &amp;&amp; context == 'love') {return 'Sometimes it takes sadness to know happiness, noise to appreciate silence and absence to value presence.';}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='sad' &amp;&amp; context == 'love') {return 'When you’re happy you enjoy the music, but when you’re sad you understand the lyrics.';}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='sad' &amp;&amp; context == 'love') {return 'Chasing happiness is guaranteed to make you unhappy.';}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='sad' &amp;&amp; context == 'work') {return 'I learned how to be happy because I know what unhappiness felt like.';}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='happy' &amp;&amp; context == 'family and friends') {return 'Happiness is not doing fun things. Happiness is doing meaningful things.';}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='happy' &amp;&amp; context == 'family and friends') {return 'One of the keys to happiness is a bad memory. ';}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='happy' &amp;&amp; context == 'family and friends') {return 'He who lives in harmony with himself lives in harmony with the universe. ';}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='happy' &amp;&amp; context == 'family and friends') {return 'Happiness is a state where nothing is missing.';}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='happy' &amp;&amp; context == 'family and friends') {return 'Three grand essentials to happiness in this life are something to do, something to love, and something to hope for. ';}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='happy' &amp;&amp; context == 'family and friends') {return 'Happiness is a function of accepting what is.';}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='stress' &amp;&amp; context == 'work') {return 'When I look back on all these worries, I remember the story of the old man who said on his deathbed that he had had a lot of trouble in his life, most of which had never happened.';}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='stress' &amp;&amp; context == 'work') {return 'Remember that stress doesn’t come from what’s going on in your life. It comes from your thoughts about what’s going on in your life.';}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='stress' &amp;&amp; context == 'work') {return 'You are braver than you believe, and stronger than you seem, and smarter than you think.';}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='stress' &amp;&amp; context == 'work') {return 'The greatest weapon against stress is our ability to choose one thought over another.';}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='stress' &amp;&amp; context == 'work') {return 'You will never change your life until you change something you do daily.';}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" t="s">
-        <v>28</v>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>else if(feeling =='stress' &amp;&amp; context == 'work') {return 'When we long for life without difficulties, remind us that oaks grow strong in contrary winds and diamonds are made under pressure.';}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>